<commit_message>
separated css and js into separate files. Completed formatting for HP bar
</commit_message>
<xml_diff>
--- a/Game Layout.xlsx
+++ b/Game Layout.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Hangman title</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>Footer</t>
+  </si>
+  <si>
+    <t>Play</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>60|100</t>
   </si>
 </sst>
 </file>
@@ -82,15 +91,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -178,11 +193,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -193,6 +260,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -217,15 +287,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,124 +582,124 @@
   <dimension ref="I6:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X33" sqref="X33"/>
+      <selection activeCell="I6" sqref="I6:V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="6" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="12"/>
     </row>
     <row r="7" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I7" s="12"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="14"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="15"/>
     </row>
     <row r="8" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I8" s="12"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="14"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="15"/>
     </row>
     <row r="9" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="17"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="18"/>
     </row>
     <row r="10" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="12"/>
       <c r="U10" s="5"/>
       <c r="V10" s="6"/>
     </row>
     <row r="11" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="14"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="15"/>
       <c r="U11" s="5"/>
       <c r="V11" s="6"/>
     </row>
     <row r="12" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="17"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="18"/>
       <c r="U12" s="5"/>
       <c r="V12" s="6"/>
     </row>
@@ -682,7 +755,7 @@
       <c r="U15" s="5"/>
       <c r="V15" s="6"/>
     </row>
-    <row r="16" spans="9:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="9:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I16" s="4"/>
       <c r="J16" s="5"/>
       <c r="K16" s="4"/>
@@ -702,12 +775,13 @@
       <c r="U16" s="5"/>
       <c r="V16" s="6"/>
     </row>
-    <row r="17" spans="9:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I17" s="4"/>
       <c r="J17" s="5"/>
       <c r="K17" s="4"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="22"/>
       <c r="O17" s="5"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="5"/>
@@ -721,7 +795,9 @@
       <c r="I18" s="4"/>
       <c r="J18" s="5"/>
       <c r="K18" s="4"/>
-      <c r="L18" s="5"/>
+      <c r="L18" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
@@ -753,8 +829,12 @@
       <c r="I20" s="4"/>
       <c r="J20" s="5"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
+      <c r="L20" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" s="21" t="s">
+        <v>8</v>
+      </c>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="4"/>
@@ -862,54 +942,54 @@
       <c r="V26" s="6"/>
     </row>
     <row r="27" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I27" s="20" t="s">
+      <c r="I27" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
-      <c r="T27" s="10"/>
-      <c r="U27" s="10"/>
-      <c r="V27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="12"/>
     </row>
     <row r="28" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I28" s="12"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13"/>
-      <c r="U28" s="13"/>
-      <c r="V28" s="14"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14"/>
+      <c r="T28" s="14"/>
+      <c r="U28" s="14"/>
+      <c r="V28" s="15"/>
     </row>
     <row r="29" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I29" s="15"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="16"/>
-      <c r="T29" s="16"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="17"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="17"/>
+      <c r="T29" s="17"/>
+      <c r="U29" s="17"/>
+      <c r="V29" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Merged function for board update and incorrect letter array
</commit_message>
<xml_diff>
--- a/Game Layout.xlsx
+++ b/Game Layout.xlsx
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Hangman title</t>
   </si>
   <si>
     <t xml:space="preserve">Game title wins description </t>
-  </si>
-  <si>
-    <t>Game directions</t>
   </si>
   <si>
     <t>HP meter</t>
@@ -54,7 +51,7 @@
     <t>Reset</t>
   </si>
   <si>
-    <t>60|100</t>
+    <t>Game directions: lkjasldjalsjdlajsldjal</t>
   </si>
 </sst>
 </file>
@@ -91,7 +88,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,6 +98,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -260,6 +263,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -293,12 +299,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,124 +585,124 @@
   <dimension ref="I6:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:V29"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="6" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="13"/>
     </row>
     <row r="7" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I7" s="13"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="15"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="16"/>
     </row>
     <row r="8" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I8" s="13"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="15"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="16"/>
     </row>
     <row r="9" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I9" s="16"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="17"/>
-      <c r="V9" s="18"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="19"/>
     </row>
     <row r="10" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="20" t="s">
+      <c r="K10" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="13"/>
       <c r="U10" s="5"/>
       <c r="V10" s="6"/>
     </row>
     <row r="11" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="15"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="16"/>
       <c r="U11" s="5"/>
       <c r="V11" s="6"/>
     </row>
     <row r="12" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="18"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="19"/>
       <c r="U12" s="5"/>
       <c r="V12" s="6"/>
     </row>
@@ -740,14 +743,14 @@
       <c r="J15" s="5"/>
       <c r="K15" s="4"/>
       <c r="L15" s="5" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
@@ -755,19 +758,14 @@
       <c r="U15" s="5"/>
       <c r="V15" s="6"/>
     </row>
-    <row r="16" spans="9:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I16" s="4"/>
       <c r="J16" s="5"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
@@ -775,13 +773,10 @@
       <c r="U16" s="5"/>
       <c r="V16" s="6"/>
     </row>
-    <row r="17" spans="9:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I17" s="4"/>
       <c r="J17" s="5"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="22"/>
       <c r="O17" s="5"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="5"/>
@@ -791,12 +786,12 @@
       <c r="U17" s="5"/>
       <c r="V17" s="6"/>
     </row>
-    <row r="18" spans="9:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I18" s="4"/>
       <c r="J18" s="5"/>
       <c r="K18" s="4"/>
       <c r="L18" s="5" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
@@ -809,13 +804,13 @@
       <c r="U18" s="5"/>
       <c r="V18" s="6"/>
     </row>
-    <row r="19" spans="9:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I19" s="4"/>
       <c r="J19" s="5"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="24"/>
       <c r="O19" s="5"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="5"/>
@@ -829,12 +824,8 @@
       <c r="I20" s="4"/>
       <c r="J20" s="5"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="M20" s="21" t="s">
-        <v>8</v>
-      </c>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="4"/>
@@ -865,8 +856,12 @@
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
+      <c r="L22" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="M22" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="4"/>
@@ -942,54 +937,54 @@
       <c r="V26" s="6"/>
     </row>
     <row r="27" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I27" s="19" t="s">
-        <v>6</v>
+      <c r="I27" s="20" t="s">
+        <v>5</v>
       </c>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-      <c r="S27" s="11"/>
-      <c r="T27" s="11"/>
-      <c r="U27" s="11"/>
-      <c r="V27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="13"/>
     </row>
     <row r="28" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I28" s="13"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="14"/>
-      <c r="U28" s="14"/>
-      <c r="V28" s="15"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
+      <c r="T28" s="15"/>
+      <c r="U28" s="15"/>
+      <c r="V28" s="16"/>
     </row>
     <row r="29" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I29" s="16"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17"/>
-      <c r="Q29" s="17"/>
-      <c r="R29" s="17"/>
-      <c r="S29" s="17"/>
-      <c r="T29" s="17"/>
-      <c r="U29" s="17"/>
-      <c r="V29" s="18"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18"/>
+      <c r="U29" s="18"/>
+      <c r="V29" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>